<commit_message>
feat(global archives): global archives created
global archives created on each table
</commit_message>
<xml_diff>
--- a/assets/streaming_ data_dictionary.xlsx
+++ b/assets/streaming_ data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.fraisse\Documents\Simplon\Projects\streaming-PF\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3567F2-7B94-47F1-8F9A-632665F320A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60B4CC9-FBF1-49A8-BCEF-F72571863301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="74">
   <si>
     <t>users</t>
   </si>
@@ -226,6 +226,27 @@
   </si>
   <si>
     <t>Targets the user column that has been changed</t>
+  </si>
+  <si>
+    <t>creationDate</t>
+  </si>
+  <si>
+    <t>TimeStamp</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd HH:mm:ss.fffffff</t>
+  </si>
+  <si>
+    <t>Set the date and time of the row's creation</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Set the date and time of the last row's update</t>
+  </si>
+  <si>
+    <t>userUpdateDate</t>
   </si>
 </sst>
 </file>
@@ -257,7 +278,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -352,17 +373,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -386,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -397,12 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -414,6 +419,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,18 +701,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.20703125" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" customWidth="1"/>
+    <col min="2" max="2" width="14.26171875" customWidth="1"/>
     <col min="3" max="3" width="11.05078125" customWidth="1"/>
-    <col min="4" max="4" width="11.89453125" customWidth="1"/>
+    <col min="4" max="4" width="25.47265625" customWidth="1"/>
     <col min="5" max="6" width="16.5234375" customWidth="1"/>
     <col min="7" max="7" width="40.68359375" customWidth="1"/>
   </cols>
@@ -746,7 +753,7 @@
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F2" t="s">
@@ -764,7 +771,7 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>50</v>
       </c>
       <c r="F3" t="s">
@@ -782,7 +789,7 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>50</v>
       </c>
       <c r="F4" t="s">
@@ -803,7 +810,7 @@
       <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="10"/>
       <c r="F5" t="s">
         <v>39</v>
       </c>
@@ -812,72 +819,64 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="13">
+      <c r="D6" s="14"/>
+      <c r="E6" s="15">
         <v>50</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="F6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>42</v>
+      <c r="B7" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13">
-        <v>50</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>56</v>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>23</v>
@@ -885,346 +884,598 @@
       <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15">
+        <v>50</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="7"/>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7"/>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="E14" s="10"/>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="12">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="7"/>
-      <c r="B12" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18">
-        <v>50</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="13">
-        <v>50</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>50</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15">
+        <v>50</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15">
+        <v>50</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="7"/>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="10">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="7"/>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="7"/>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="12">
-        <v>50</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13">
-        <v>50</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="7"/>
+      <c r="B27" t="s">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E27" s="10">
         <v>50</v>
       </c>
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="8" t="s">
+      <c r="F27" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15">
+        <v>50</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7"/>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="10">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="7"/>
-      <c r="B23" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="7"/>
+      <c r="B33" t="s">
         <v>3</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E33" s="10">
         <v>50</v>
       </c>
-      <c r="F23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="E34" s="15"/>
+      <c r="F34" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="4" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E37" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="F37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C38" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="13">
+      <c r="D38" s="14"/>
+      <c r="E38" s="15">
         <v>50</v>
       </c>
-      <c r="F26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="11" t="s">
+      <c r="F38" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="8" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="14"/>
+      <c r="B39" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="9"/>
+      <c r="B40" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>